<commit_message>
sửa lại file excel du lieu sinh  vien va them danh sach
</commit_message>
<xml_diff>
--- a/Design document/Excels/dang_vien.xlsx
+++ b/Design document/Excels/dang_vien.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="36">
   <si>
     <t xml:space="preserve">id</t>
   </si>
@@ -40,7 +40,7 @@
     <t xml:space="preserve">dang_vien</t>
   </si>
   <si>
-    <t xml:space="preserve">Lều Văn Duẩn</t>
+    <t xml:space="preserve">Nguyễn Hữu Hồng</t>
   </si>
   <si>
     <t xml:space="preserve">K59CA</t>
@@ -49,106 +49,85 @@
     <t xml:space="preserve">Đảng Viên</t>
   </si>
   <si>
-    <t xml:space="preserve">Nguyễn Trọng Đông</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Trường Giang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Hữu Hồng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Tiến Việt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K59CAC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bùi Tiến Đạt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phạm Văn Định</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Trung Hiếu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">14020022</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Hoàng Biên</t>
+    <t xml:space="preserve">Nguyễn Như Huy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lương Ngọc Huyền</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Quang Bách</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K59CB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dương Công Đại</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Châu Quốc Đạt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dương Xuân Đồng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trần Việt Đức</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Thị Hồng Hải</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Văn Hải</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Thị Hạnh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hoàng Thanh Hằng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bùi Duy Hiển</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Mạnh Cường</t>
   </si>
   <si>
     <t xml:space="preserve">K59CLC</t>
   </si>
   <si>
-    <t xml:space="preserve">Nguyễn Thành Công</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bùi Quang Cường</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Mạnh Cường</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trần Văn An</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K59CB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hoàng Tuấn Anh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Hoàng Anh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Quang Bách</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lê Đức Duy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K59CC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Ngọc Duy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trịnh Quốc Đạt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lương Văn Đông</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lê Đình Dũng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K59CD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ngô Tùng Dương</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Minh Dương</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vũ Đình Đúng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Minh Công</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K59N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trần Thị Dung</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nguyễn Việt Dũng</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Phạm Tùng Dương</t>
+    <t xml:space="preserve">Hà Hồng Duyên</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trần Đình Dương</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Văn Đại</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trần Thị Thanh Huyền</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phạm Quang Hưng</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Đức Khanh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Thị Lan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phạm Minh Hoàng Linh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vũ Thùy Linh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nguyễn Việt Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tô Hiến Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Đinh Tiến Lộc</t>
   </si>
 </sst>
 </file>
@@ -159,7 +138,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="M/D/YYYY"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -191,12 +170,6 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
@@ -257,7 +230,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -274,26 +247,18 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -306,24 +271,8 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -347,18 +296,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F27"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H24" activeCellId="0" sqref="H24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0918367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -386,13 +333,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>14020062</v>
+        <v>14020198</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D2" s="4" t="n">
-        <v>34704</v>
+        <v>35347</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>7</v>
@@ -406,13 +353,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>14020791</v>
+        <v>14020208</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="5" t="n">
-        <v>35290</v>
+      <c r="D3" s="4" t="n">
+        <v>35209</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>7</v>
@@ -426,13 +373,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>14020783</v>
+        <v>14020664</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="5" t="n">
-        <v>35345</v>
+      <c r="D4" s="4" t="n">
+        <v>35207</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>7</v>
@@ -446,16 +393,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>14020198</v>
-      </c>
-      <c r="C5" s="3" t="s">
+        <v>14020652</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="5" t="n">
-        <v>35347</v>
+      <c r="D5" s="6" t="n">
+        <v>35176</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F5" s="0" t="s">
         <v>8</v>
@@ -465,17 +412,17 @@
       <c r="A6" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="6" t="n">
-        <v>14020553</v>
-      </c>
-      <c r="C6" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="5" t="n">
-        <v>35282</v>
+      <c r="B6" s="2" t="n">
+        <v>14020088</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="6" t="n">
+        <v>35375</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F6" s="0" t="s">
         <v>8</v>
@@ -486,16 +433,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>14020581</v>
-      </c>
-      <c r="C7" s="8" t="s">
+        <v>14020582</v>
+      </c>
+      <c r="C7" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="5" t="n">
-        <v>35137</v>
+      <c r="D7" s="6" t="n">
+        <v>35289</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" s="0" t="s">
         <v>8</v>
@@ -506,16 +453,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>14020108</v>
-      </c>
-      <c r="C8" s="8" t="s">
+        <v>14020116</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="5" t="n">
-        <v>35104</v>
+      <c r="D8" s="6" t="n">
+        <v>35226</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F8" s="0" t="s">
         <v>8</v>
@@ -526,276 +473,276 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>14020171</v>
-      </c>
-      <c r="C9" s="3" t="s">
+        <v>14020658</v>
+      </c>
+      <c r="C9" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="5" t="n">
-        <v>35096</v>
+      <c r="D9" s="6" t="n">
+        <v>35429</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F9" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="9" t="s">
+      <c r="B10" s="2" t="n">
+        <v>14020585</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="11" t="n">
-        <v>35332</v>
+      <c r="D10" s="6" t="n">
+        <v>35236</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F10" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="9" t="n">
-        <v>14020042</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="D11" s="11" t="n">
-        <v>35120</v>
+      <c r="B11" s="2" t="n">
+        <v>14020146</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="D11" s="6" t="n">
+        <v>35362</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F11" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="9" t="n">
-        <v>14020577</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" s="11" t="n">
-        <v>35421</v>
+      <c r="B12" s="2" t="n">
+        <v>14020661</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D12" s="6" t="n">
+        <v>35151</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F12" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="9" t="n">
-        <v>14020056</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="D13" s="11" t="n">
-        <v>35069</v>
+      <c r="B13" s="2" t="n">
+        <v>14020155</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="6" t="n">
+        <v>35212</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
       <c r="F13" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="2" t="n">
-        <v>14020002</v>
-      </c>
-      <c r="C14" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="12" t="n">
-        <v>35321</v>
+        <v>14020161</v>
+      </c>
+      <c r="C14" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="6" t="n">
+        <v>34823</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="F14" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="37.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="2" t="n">
-        <v>14020003</v>
+      <c r="B15" s="7" t="n">
+        <v>14020056</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D15" s="12" t="n">
-        <v>35126</v>
+        <v>22</v>
+      </c>
+      <c r="D15" s="9" t="n">
+        <v>35069</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="2" t="n">
-        <v>14020005</v>
+      <c r="B16" s="7" t="n">
+        <v>14020066</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="D16" s="12" t="n">
-        <v>34746</v>
+        <v>24</v>
+      </c>
+      <c r="D16" s="9" t="n">
+        <v>35376</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F16" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="2" t="n">
-        <v>14020652</v>
+      <c r="B17" s="7" t="n">
+        <v>14020084</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" s="12" t="n">
-        <v>35176</v>
+        <v>25</v>
+      </c>
+      <c r="D17" s="9" t="n">
+        <v>35300</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="13" t="n">
-        <v>14020655</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="14" t="n">
-        <v>35413</v>
+      <c r="B18" s="7" t="n">
+        <v>14020091</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="D18" s="9" t="n">
+        <v>35355</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F18" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="13" t="n">
-        <v>14020065</v>
-      </c>
-      <c r="C19" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D19" s="14" t="n">
-        <v>35348</v>
+      <c r="B19" s="2" t="n">
+        <v>14020213</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="9" t="n">
+        <v>35197</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F19" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="13" t="n">
-        <v>14020103</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="14" t="n">
-        <v>35394</v>
+      <c r="B20" s="7" t="n">
+        <v>14020225</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D20" s="9" t="n">
+        <v>35072</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F20" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="13" t="n">
-        <v>14020113</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="D21" s="14" t="n">
-        <v>34717</v>
+      <c r="B21" s="7" t="n">
+        <v>14020234</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="9" t="n">
+        <v>35120</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="F21" s="0" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="15" t="n">
-        <v>14020071</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="D22" s="16" t="n">
-        <v>35271</v>
+      <c r="B22" s="2" t="n">
+        <v>14020249</v>
+      </c>
+      <c r="C22" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D22" s="9" t="n">
+        <v>35414</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F22" s="0" t="s">
         <v>8</v>
@@ -805,17 +752,17 @@
       <c r="A23" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="15" t="n">
-        <v>14020080</v>
-      </c>
-      <c r="C23" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D23" s="16" t="n">
+      <c r="B23" s="10" t="n">
+        <v>14020752</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="9" t="n">
         <v>35373</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F23" s="0" t="s">
         <v>8</v>
@@ -825,17 +772,17 @@
       <c r="A24" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="15" t="n">
-        <v>14020657</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="D24" s="16" t="n">
-        <v>35145</v>
+      <c r="B24" s="7" t="n">
+        <v>14020629</v>
+      </c>
+      <c r="C24" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="9" t="n">
+        <v>35141</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F24" s="0" t="s">
         <v>8</v>
@@ -845,17 +792,17 @@
       <c r="A25" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="15" t="n">
-        <v>14020117</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D25" s="16" t="n">
-        <v>32470</v>
+      <c r="B25" s="7" t="n">
+        <v>14020669</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="D25" s="9" t="n">
+        <v>35383</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F25" s="0" t="s">
         <v>8</v>
@@ -865,17 +812,17 @@
       <c r="A26" s="1" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="15" t="n">
-        <v>14020041</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>38</v>
-      </c>
-      <c r="D26" s="16" t="n">
-        <v>35325</v>
+      <c r="B26" s="7" t="n">
+        <v>14020266</v>
+      </c>
+      <c r="C26" s="8" t="s">
+        <v>34</v>
+      </c>
+      <c r="D26" s="9" t="n">
+        <v>35145</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F26" s="0" t="s">
         <v>8</v>
@@ -885,59 +832,19 @@
       <c r="A27" s="1" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="15" t="n">
-        <v>14020580</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="D27" s="16" t="n">
-        <v>35359</v>
+      <c r="B27" s="7" t="n">
+        <v>14020268</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="D27" s="9" t="n">
+        <v>35419</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>39</v>
+        <v>23</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1" t="n">
-        <v>27</v>
-      </c>
-      <c r="B28" s="15" t="n">
-        <v>14020076</v>
-      </c>
-      <c r="C28" s="17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D28" s="16" t="n">
-        <v>35308</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="25.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1" t="n">
-        <v>28</v>
-      </c>
-      <c r="B29" s="15" t="n">
-        <v>14020083</v>
-      </c>
-      <c r="C29" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D29" s="16" t="n">
-        <v>35222</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F29" s="0" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>